<commit_message>
Updates for midair collisions
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/sample_inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/sample_inputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://purdue0-my.sharepoint.com/personal/chaoh_purdue_edu/Documents/AAE560/AAE560_Spring2018/DAF_Project/+airtaxi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmyers\Desktop\Air Taxi Model_032018\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{12AB5E58-326B-49BC-8A82-6448E3FF9108}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="945" yWindow="465" windowWidth="28800" windowHeight="12300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operator" sheetId="3" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Chargers" sheetId="4" r:id="rId4"/>
     <sheet name="Pricing" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Team ID</t>
   </si>
@@ -112,9 +113,6 @@
   </si>
   <si>
     <t>Charging Rate (mile range/min)</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Yes</t>
@@ -144,7 +142,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -542,25 +540,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
-    <col min="10" max="10" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,21 +565,21 @@
         <v>1</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -591,31 +588,31 @@
       </c>
       <c r="C3" s="1"/>
       <c r="J3" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="10">
         <f>B15+B11</f>
-        <v>960000</v>
+        <v>2780000</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="10">
         <f>B3-B4</f>
-        <v>540000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+        <v>-1280000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -632,37 +629,37 @@
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="11">
         <f>C10+D10</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C10" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="10">
         <f>C10*Aircraft!E2 + D10*Aircraft!E3  + E10*Aircraft!E4</f>
-        <v>800000</v>
+        <v>2600000</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="str">
         <f>IF(Ports!A2="","","Port "&amp;Ports!A2)</f>
         <v>Port 1</v>
@@ -710,25 +707,25 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="12">
         <f>COUNTIF(C13:G13,"Yes")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>28</v>
@@ -741,7 +738,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -768,56 +765,56 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="10">
         <f>IF(C14=Chargers!A2,Chargers!C2,IF(C14=Chargers!A3,Chargers!C3,0))*IF(C13="Yes",1,0)+IF(D14=Chargers!A2,Chargers!C2,IF(D14=Chargers!A3,Chargers!C3,0))*IF(D13="Yes",1,0)+IF(E14=Chargers!A2,Chargers!C2,IF(E14=Chargers!A3,Chargers!C3,0))*IF(E13="Yes",1,0)+IF(F14=Chargers!A2,Chargers!C2,IF(F14=Chargers!A3,Chargers!C3,0))*IF(F13="Yes",1,0)+IF(G14=Chargers!A2,Chargers!C2,IF(G14=Chargers!A3,Chargers!C3,0))*IF(G13="Yes",1,0)</f>
-        <v>160000</v>
+        <v>180000</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="8:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H18" s="6"/>
       <c r="I18" s="7"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="8:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="8:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="8:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:N13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:N13" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:G14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:G14" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Slow, Fast, None"</formula1>
     </dataValidation>
   </dataValidations>
@@ -827,23 +824,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -860,7 +857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -877,7 +874,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -894,10 +891,10 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
   </sheetData>
@@ -907,25 +904,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="4" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1796875" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="2" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -946,7 +941,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -960,13 +955,13 @@
         <v>0.2</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F2" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -980,13 +975,13 @@
         <v>0.3</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1000,13 +995,13 @@
         <v>0.1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1020,13 +1015,13 @@
         <v>0.4</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1040,7 +1035,7 @@
         <v>0.6</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6" s="9">
         <v>20</v>
@@ -1052,21 +1047,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1082,7 +1077,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1093,7 +1088,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1110,20 +1105,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1131,7 +1126,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(ISBLANK(Aircraft!A2),"",Aircraft!A2)</f>
         <v>Type 1</v>
@@ -1140,7 +1135,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF(ISBLANK(Aircraft!A3),"",Aircraft!A3)</f>
         <v>Type 2</v>
@@ -1149,119 +1144,119 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF(ISBLANK(Aircraft!A4),"",Aircraft!A4)</f>
         <v/>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF(ISBLANK(Aircraft!A5),"",Aircraft!A5)</f>
         <v/>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(ISBLANK(Aircraft!A6),"",Aircraft!A6)</f>
         <v/>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF(ISBLANK(Aircraft!A7),"",Aircraft!A7)</f>
         <v/>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF(ISBLANK(Aircraft!A8),"",Aircraft!A8)</f>
         <v/>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF(ISBLANK(Aircraft!A9),"",Aircraft!A9)</f>
         <v/>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF(ISBLANK(Aircraft!A10),"",Aircraft!A10)</f>
         <v/>
       </c>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF(ISBLANK(Aircraft!A11),"",Aircraft!A11)</f>
         <v/>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF(ISBLANK(Aircraft!A12),"",Aircraft!A12)</f>
         <v/>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF(ISBLANK(Aircraft!A13),"",Aircraft!A13)</f>
         <v/>
       </c>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF(ISBLANK(Aircraft!A14),"",Aircraft!A14)</f>
         <v/>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF(ISBLANK(Aircraft!A15),"",Aircraft!A15)</f>
         <v/>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF(ISBLANK(Aircraft!A16),"",Aircraft!A16)</f>
         <v/>
       </c>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF(ISBLANK(Aircraft!A17),"",Aircraft!A17)</f>
         <v/>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF(ISBLANK(Aircraft!A18),"",Aircraft!A18)</f>
         <v/>
       </c>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF(ISBLANK(Aircraft!A19),"",Aircraft!A19)</f>
         <v/>
       </c>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF(ISBLANK(Aircraft!A20),"",Aircraft!A20)</f>
         <v/>

</xml_diff>

<commit_message>
added nav and avoidance for datalinks
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/sample_inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/sample_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmyers\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{39F9B85B-43C6-4300-BD67-2262E1E5FD2C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{76AF9BA4-09FE-4C63-A825-01432E2C5BE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="465" windowWidth="28800" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4725" yWindow="465" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operator" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Team ID</t>
   </si>
@@ -543,17 +543,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="3" max="8" width="7.85546875" customWidth="1"/>
     <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -597,7 +593,7 @@
       </c>
       <c r="B4" s="10">
         <f>B15+B11</f>
-        <v>2780000</v>
+        <v>4980000</v>
       </c>
       <c r="J4" s="19" t="s">
         <v>35</v>
@@ -609,7 +605,7 @@
       </c>
       <c r="B6" s="10">
         <f>B3-B4</f>
-        <v>-1280000</v>
+        <v>-3480000</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -635,13 +631,13 @@
       </c>
       <c r="B10" s="11">
         <f>C10+D10</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C10" s="13">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D10" s="13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -653,7 +649,7 @@
       </c>
       <c r="B11" s="10">
         <f>C10*Aircraft!E2 + D10*Aircraft!E3  + E10*Aircraft!E4</f>
-        <v>2600000</v>
+        <v>4800000</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -682,7 +678,7 @@
       </c>
       <c r="H12" s="1" t="str">
         <f>IF(Ports!A7="","","Port "&amp;Ports!A7)</f>
-        <v/>
+        <v>Port 6</v>
       </c>
       <c r="I12" s="1" t="str">
         <f>IF(Ports!A8="","","Port "&amp;Ports!A8)</f>
@@ -712,8 +708,8 @@
         <v>19</v>
       </c>
       <c r="B13" s="12">
-        <f>COUNTIF(C13:G13,"Yes")</f>
-        <v>5</v>
+        <f>COUNTIF(C13:I13,"Yes")</f>
+        <v>6</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>28</v>
@@ -730,7 +726,9 @@
       <c r="G13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -761,7 +759,9 @@
       <c r="G14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
@@ -814,7 +814,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:N13" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:G14" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:H14" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Slow, Fast, None"</formula1>
     </dataValidation>
   </dataValidations>
@@ -827,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -905,7 +905,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -955,7 +955,7 @@
         <v>0.2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2" s="9">
         <v>20</v>
@@ -975,7 +975,7 @@
         <v>0.3</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F3" s="9">
         <v>20</v>
@@ -995,7 +995,7 @@
         <v>0.1</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F4" s="9">
         <v>20</v>
@@ -1015,7 +1015,7 @@
         <v>0.4</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F5" s="9">
         <v>20</v>
@@ -1035,9 +1035,29 @@
         <v>0.6</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F6" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>72</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="9">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reset aircraft after crashes and log
Logs crashes and resets the aircraft.
Data processing evaluates the number of crashes.
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/sample_inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/sample_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmyers\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{76AF9BA4-09FE-4C63-A825-01432E2C5BE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BDBF308A-64BC-44C4-8954-1796CD3B0D9B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="465" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="465" windowWidth="28800" windowHeight="12300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operator" sheetId="3" r:id="rId1"/>
@@ -543,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -827,9 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -862,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -879,7 +877,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="C3">
         <v>200</v>
@@ -905,9 +903,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -916,11 +914,9 @@
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -939,9 +935,8 @@
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -961,7 +956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -981,7 +976,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1001,7 +996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1021,7 +1016,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1041,7 +1036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Latest updates from master
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/sample_inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/sample_inputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://purdue0-my.sharepoint.com/personal/chaoh_purdue_edu/Documents/AAE560/AAE560_Spring2018/DAF_Project/+airtaxi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmyers\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BDBF308A-64BC-44C4-8954-1796CD3B0D9B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="7560" yWindow="465" windowWidth="28800" windowHeight="12300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operator" sheetId="3" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Chargers" sheetId="4" r:id="rId4"/>
     <sheet name="Pricing" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Team ID</t>
   </si>
@@ -112,9 +113,6 @@
   </si>
   <si>
     <t>Charging Rate (mile range/min)</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Yes</t>
@@ -144,7 +142,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -542,25 +540,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
-    <col min="10" max="10" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,21 +561,21 @@
         <v>1</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -591,31 +584,31 @@
       </c>
       <c r="C3" s="1"/>
       <c r="J3" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="10">
         <f>B15+B11</f>
-        <v>960000</v>
+        <v>4980000</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="10">
         <f>B3-B4</f>
-        <v>540000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+        <v>-3480000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -632,37 +625,37 @@
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="11">
         <f>C10+D10</f>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C10" s="13">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D10" s="13">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="10">
         <f>C10*Aircraft!E2 + D10*Aircraft!E3  + E10*Aircraft!E4</f>
-        <v>800000</v>
+        <v>4800000</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="str">
         <f>IF(Ports!A2="","","Port "&amp;Ports!A2)</f>
         <v>Port 1</v>
@@ -685,7 +678,7 @@
       </c>
       <c r="H12" s="1" t="str">
         <f>IF(Ports!A7="","","Port "&amp;Ports!A7)</f>
-        <v/>
+        <v>Port 6</v>
       </c>
       <c r="I12" s="1" t="str">
         <f>IF(Ports!A8="","","Port "&amp;Ports!A8)</f>
@@ -710,30 +703,32 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="12">
-        <f>COUNTIF(C13:G13,"Yes")</f>
-        <v>4</v>
+        <f>COUNTIF(C13:I13,"Yes")</f>
+        <v>6</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -741,7 +736,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -764,60 +759,62 @@
       <c r="G14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="10">
         <f>IF(C14=Chargers!A2,Chargers!C2,IF(C14=Chargers!A3,Chargers!C3,0))*IF(C13="Yes",1,0)+IF(D14=Chargers!A2,Chargers!C2,IF(D14=Chargers!A3,Chargers!C3,0))*IF(D13="Yes",1,0)+IF(E14=Chargers!A2,Chargers!C2,IF(E14=Chargers!A3,Chargers!C3,0))*IF(E13="Yes",1,0)+IF(F14=Chargers!A2,Chargers!C2,IF(F14=Chargers!A3,Chargers!C3,0))*IF(F13="Yes",1,0)+IF(G14=Chargers!A2,Chargers!C2,IF(G14=Chargers!A3,Chargers!C3,0))*IF(G13="Yes",1,0)</f>
-        <v>160000</v>
+        <v>180000</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="8:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H18" s="6"/>
       <c r="I18" s="7"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="8:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="8:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="8:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:N13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:N13" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:G14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:H14" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Slow, Fast, None"</formula1>
     </dataValidation>
   </dataValidations>
@@ -827,23 +824,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -860,12 +855,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -877,12 +872,12 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="C3">
         <v>200</v>
@@ -894,10 +889,10 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
   </sheetData>
@@ -907,25 +902,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="4" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1796875" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="2" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -944,9 +935,8 @@
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -960,13 +950,13 @@
         <v>0.2</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -980,13 +970,13 @@
         <v>0.3</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F3" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1000,13 +990,13 @@
         <v>0.1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1020,13 +1010,13 @@
         <v>0.4</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F5" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1040,9 +1030,29 @@
         <v>0.6</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>72</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="9">
         <v>20</v>
       </c>
     </row>
@@ -1052,21 +1062,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1082,7 +1092,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1093,7 +1103,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1110,20 +1120,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1131,7 +1141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(ISBLANK(Aircraft!A2),"",Aircraft!A2)</f>
         <v>Type 1</v>
@@ -1140,7 +1150,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF(ISBLANK(Aircraft!A3),"",Aircraft!A3)</f>
         <v>Type 2</v>
@@ -1149,119 +1159,119 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF(ISBLANK(Aircraft!A4),"",Aircraft!A4)</f>
         <v/>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF(ISBLANK(Aircraft!A5),"",Aircraft!A5)</f>
         <v/>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(ISBLANK(Aircraft!A6),"",Aircraft!A6)</f>
         <v/>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF(ISBLANK(Aircraft!A7),"",Aircraft!A7)</f>
         <v/>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF(ISBLANK(Aircraft!A8),"",Aircraft!A8)</f>
         <v/>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF(ISBLANK(Aircraft!A9),"",Aircraft!A9)</f>
         <v/>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF(ISBLANK(Aircraft!A10),"",Aircraft!A10)</f>
         <v/>
       </c>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF(ISBLANK(Aircraft!A11),"",Aircraft!A11)</f>
         <v/>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF(ISBLANK(Aircraft!A12),"",Aircraft!A12)</f>
         <v/>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF(ISBLANK(Aircraft!A13),"",Aircraft!A13)</f>
         <v/>
       </c>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF(ISBLANK(Aircraft!A14),"",Aircraft!A14)</f>
         <v/>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF(ISBLANK(Aircraft!A15),"",Aircraft!A15)</f>
         <v/>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF(ISBLANK(Aircraft!A16),"",Aircraft!A16)</f>
         <v/>
       </c>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF(ISBLANK(Aircraft!A17),"",Aircraft!A17)</f>
         <v/>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF(ISBLANK(Aircraft!A18),"",Aircraft!A18)</f>
         <v/>
       </c>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF(ISBLANK(Aircraft!A19),"",Aircraft!A19)</f>
         <v/>
       </c>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF(ISBLANK(Aircraft!A20),"",Aircraft!A20)</f>
         <v/>

</xml_diff>